<commit_message>
Add new template file for front-end JS codes.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="181">
   <si>
     <t>SeqNo</t>
   </si>
@@ -275,406 +275,458 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>tbDscr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isExist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>經辦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代碼設定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeqNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代碼分類</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>orderBy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>異動者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>異動時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>queryWhere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>httpUpdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDate()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aux</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>休息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aux</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>休息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A02344</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daniel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0034</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>334</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0930744573</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daniel@esun.bank.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>httpInsert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>職務權限設定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/admin/auth/index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fm-icon-home</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PcPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分機號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電腦名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電腦IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PcPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電腦電話</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A02344</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroupId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memo1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>httpGet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColDscr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統代碼檔代碼</t>
+  </si>
+  <si>
+    <t>系統代碼檔名稱</t>
+  </si>
+  <si>
+    <t>功能路由</t>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否啟用?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc-phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>tableName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>User</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Func</t>
-  </si>
-  <si>
-    <t>tbDscr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>系統代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isExist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>agent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>經辦</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代碼設定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SeqNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代碼分類</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>orderBy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateDT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>異動者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>異動時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>queryWhere</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>httpUpdate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>getDate()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aux</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>休息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aux</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>休息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A02344</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>daniel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0034</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>334</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0930744573</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>daniel@esun.bank.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>httpInsert</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>職務權限設定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/admin/auth/index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fm-icon-home</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PcPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComputerName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComputerIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsEnable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分機號碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電腦名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電腦IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>備註</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PcPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電腦電話</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0033</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A02344</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GroupId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CP0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memo1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A0023</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>httpGet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nvarchar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Column</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColDscr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>系統代碼檔代碼</t>
-  </si>
-  <si>
-    <t>系統代碼檔名稱</t>
-  </si>
-  <si>
-    <t>功能路由</t>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否啟用?</t>
+    <t>table_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>computerName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>computerIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isEnable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createDT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateDT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>codeName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isEnable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1147,7 +1199,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1157,9 +1209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O60" sqref="O60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1194,10 +1246,10 @@
         <v>19</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>13</v>
@@ -1215,22 +1267,22 @@
         <v>56</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1256,13 +1308,13 @@
         <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="16">
         <v>2</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="O2" s="16"/>
     </row>
@@ -1280,28 +1332,28 @@
         <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G3" s="3">
         <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1312,7 +1364,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>24</v>
@@ -1327,13 +1379,13 @@
         <v>57</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1344,7 +1396,7 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>25</v>
@@ -1359,19 +1411,19 @@
         <v>57</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1394,13 +1446,13 @@
         <v>20</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1411,7 +1463,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>27</v>
@@ -1423,16 +1475,16 @@
         <v>20</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1455,16 +1507,16 @@
         <v>10</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1490,16 +1542,16 @@
         <v>12</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1525,13 +1577,13 @@
         <v>12</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1571,10 +1623,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M12" s="26">
         <v>1</v>
@@ -1606,7 +1658,7 @@
         <v>7</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1640,7 +1692,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>36</v>
@@ -1649,7 +1701,7 @@
         <v>20</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1660,7 +1712,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>32</v>
@@ -1672,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1686,7 +1738,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>38</v>
@@ -1746,28 +1798,28 @@
         <v>40</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G19" s="3">
         <v>20</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L19" s="16">
         <v>1</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1790,22 +1842,22 @@
         <v>50</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1819,7 +1871,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>35</v>
@@ -1828,13 +1880,13 @@
         <v>20</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1857,13 +1909,13 @@
         <v>20</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1877,10 +1929,10 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M23" s="26">
         <v>1</v>
@@ -1923,7 +1975,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>36</v>
@@ -1932,7 +1984,7 @@
         <v>20</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1943,7 +1995,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>32</v>
@@ -1955,7 +2007,7 @@
         <v>7</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1969,7 +2021,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>38</v>
@@ -2029,28 +2081,28 @@
         <v>63</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G29" s="3">
         <v>20</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L29" s="16">
         <v>1</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2073,22 +2125,22 @@
         <v>50</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2102,10 +2154,10 @@
         <v>7</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M31" s="26">
         <v>1</v>
@@ -2148,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>36</v>
@@ -2157,7 +2209,7 @@
         <v>20</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2168,7 +2220,7 @@
         <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>32</v>
@@ -2180,7 +2232,7 @@
         <v>7</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2194,7 +2246,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>38</v>
@@ -2204,7 +2256,7 @@
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -2254,31 +2306,31 @@
         <v>50</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G37" s="3">
         <v>20</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L37" s="16">
         <v>1</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -2301,22 +2353,22 @@
         <v>50</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2330,10 +2382,10 @@
         <v>7</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M39" s="26">
         <v>1</v>
@@ -2378,7 +2430,7 @@
         <v>11</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>36</v>
@@ -2397,7 +2449,7 @@
         <v>49</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>32</v>
@@ -2411,7 +2463,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="6"/>
       <c r="P42" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2477,7 @@
         <v>10</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>38</v>
@@ -2435,7 +2487,7 @@
       </c>
       <c r="K43" s="8"/>
       <c r="L43" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -2446,13 +2498,13 @@
         <v>21</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>22</v>
@@ -2467,7 +2519,7 @@
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L44" s="19">
         <v>1</v>
@@ -2483,14 +2535,14 @@
         <v>21</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>35</v>
@@ -2502,22 +2554,22 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L45" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N45" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M45" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="O45" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2525,17 +2577,17 @@
         <v>21</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G46" s="5">
         <v>20</v>
@@ -2544,22 +2596,22 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L46" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N46" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M46" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="O46" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -2567,41 +2619,41 @@
         <v>21</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L47" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N47" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="M47" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="O47" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -2609,17 +2661,17 @@
         <v>21</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -2644,11 +2696,11 @@
         <v>21</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>33</v>
@@ -2667,7 +2719,7 @@
       <c r="M49" s="5"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -2675,14 +2727,14 @@
         <v>21</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>36</v>
@@ -2695,10 +2747,10 @@
       <c r="J50" s="5"/>
       <c r="K50" s="6"/>
       <c r="L50" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
@@ -2708,11 +2760,11 @@
         <v>21</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>32</v>
@@ -2737,14 +2789,14 @@
         <v>21</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>38</v>
@@ -2757,7 +2809,7 @@
       <c r="J52" s="9"/>
       <c r="K52" s="10"/>
       <c r="L52" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M52" s="9"/>
       <c r="N52" s="8"/>
@@ -2769,13 +2821,13 @@
         <v>21</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>22</v>
@@ -2790,10 +2842,10 @@
       </c>
       <c r="J53" s="21"/>
       <c r="K53" s="22" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="L53" s="23" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="M53" s="26">
         <v>1</v>
@@ -2808,13 +2860,13 @@
         <v>21</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>35</v>
@@ -2823,22 +2875,22 @@
         <v>20</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="N54" s="24" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -2846,31 +2898,31 @@
         <v>21</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -2878,37 +2930,37 @@
         <v>21</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="G56" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P56" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L56" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="P56" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -2916,28 +2968,28 @@
         <v>21</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="P57" s="2" t="s">
         <v>20</v>
@@ -2948,16 +3000,16 @@
         <v>21</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="M58" s="26">
         <v>1</v>
@@ -2966,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="O58" s="27" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -2974,10 +3026,10 @@
         <v>21</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>33</v>
@@ -2995,13 +3047,13 @@
         <v>21</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>36</v>
@@ -3010,7 +3062,7 @@
         <v>20</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -3018,10 +3070,10 @@
         <v>21</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>32</v>
@@ -3038,13 +3090,13 @@
         <v>21</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>38</v>
@@ -3074,76 +3126,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add JS/views/admin/edit-form.vue template. Done.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="186">
   <si>
     <t>SeqNo</t>
   </si>
@@ -671,10 +671,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>computerIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>memo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -731,6 +727,26 @@
   </si>
   <si>
     <t>電話分機</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>computerIp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q-input</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -782,7 +798,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +829,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -836,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -893,6 +915,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1208,11 +1231,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R59" sqref="R59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1224,17 +1247,17 @@
     <col min="5" max="5" width="17" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="3" customWidth="1"/>
-    <col min="8" max="10" width="7.5703125" style="3" customWidth="1"/>
+    <col min="8" max="10" width="7.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="3" customWidth="1"/>
-    <col min="14" max="15" width="17.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8" style="16" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="8" style="2" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" style="3" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
@@ -1283,11 +1306,14 @@
       <c r="P1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1320,7 +1346,7 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1384,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1428,7 +1454,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1457,7 +1483,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1489,7 +1515,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1521,7 +1547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1556,7 +1582,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1614,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1640,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1663,7 +1689,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -1683,7 +1709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -1706,7 +1732,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -2541,7 +2567,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>82</v>
@@ -2583,7 +2609,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>149</v>
@@ -2625,7 +2651,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>150</v>
@@ -2667,7 +2693,7 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>154</v>
@@ -2693,7 +2719,7 @@
       </c>
       <c r="P48" s="6"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>21</v>
       </c>
@@ -2702,7 +2728,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>33</v>
@@ -2724,7 +2750,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>21</v>
       </c>
@@ -2733,7 +2759,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>89</v>
@@ -2757,7 +2783,7 @@
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>21</v>
       </c>
@@ -2766,7 +2792,7 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>32</v>
@@ -2786,7 +2812,7 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>21</v>
       </c>
@@ -2795,7 +2821,7 @@
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>90</v>
@@ -2818,7 +2844,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
     </row>
-    <row r="53" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>21</v>
       </c>
@@ -2829,10 +2855,10 @@
         <v>20</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>34</v>
@@ -2857,7 +2883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>21</v>
       </c>
@@ -2891,8 +2917,11 @@
       <c r="Q54" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>21</v>
       </c>
@@ -2900,10 +2929,10 @@
         <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>145</v>
@@ -2929,8 +2958,11 @@
       <c r="P55" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>21</v>
       </c>
@@ -2941,7 +2973,7 @@
         <v>164</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>35</v>
@@ -2970,8 +3002,11 @@
       <c r="Q56" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>21</v>
       </c>
@@ -2979,10 +3014,10 @@
         <v>116</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>35</v>
@@ -3002,8 +3037,11 @@
       <c r="P57" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>21</v>
       </c>
@@ -3011,20 +3049,32 @@
         <v>116</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>33</v>
+        <v>174</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G58" s="5">
-        <v>20</v>
-      </c>
-      <c r="P58" s="6"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="19">
+        <v>1</v>
+      </c>
+      <c r="M58" s="6">
+        <v>1</v>
+      </c>
+      <c r="N58" s="6">
+        <v>1</v>
+      </c>
+      <c r="O58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>21</v>
       </c>
@@ -3032,10 +3082,10 @@
         <v>116</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>36</v>
@@ -3043,11 +3093,9 @@
       <c r="G59" s="5">
         <v>20</v>
       </c>
-      <c r="M59" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P59" s="6"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>21</v>
       </c>
@@ -3055,42 +3103,65 @@
         <v>116</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" s="5">
+        <v>20</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G61" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="5" t="s">
+      <c r="E62" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G62" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61" s="9">
-        <v>7</v>
-      </c>
-      <c r="K61" s="8"/>
-      <c r="L61" s="18"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="6" t="s">
+      <c r="K62" s="8"/>
+      <c r="L62" s="18"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3103,6 +3174,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <ignoredErrors>
+    <ignoredError sqref="R54:R56" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add WebApi/Application/IService template is done.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="183">
   <si>
     <t>UserId</t>
   </si>
@@ -467,6 +467,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -475,18 +490,187 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PcPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電腦電話</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A02344</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroupId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memo1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>httpGet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColDscr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統代碼檔代碼</t>
+  </si>
+  <si>
+    <t>系統代碼檔名稱</t>
+  </si>
+  <si>
+    <t>功能路由</t>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否啟用?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pcPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc-phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tableName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP 位址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seq No.</t>
+  </si>
+  <si>
+    <t>filterItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電話分機</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111</t>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q-input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -498,251 +682,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PcPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電腦電話</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0033</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A02344</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GroupId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CP0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memo1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A0023</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>httpGet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nvarchar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Column</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColDscr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>系統代碼檔代碼</t>
-  </si>
-  <si>
-    <t>系統代碼檔名稱</t>
-  </si>
-  <si>
-    <t>功能路由</t>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否啟用?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>group</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pcPhone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pc-phone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tableName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>table_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IP 位址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>備註</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Seq No.</t>
-  </si>
-  <si>
-    <t>filterItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電話分機</t>
+    <t>更新者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeqNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComputerName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComputerIp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExtCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsEnable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpdateDt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CodeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CodeId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CodeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>q-input</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SeqNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComputerName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComputerIp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsEnable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Updator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateDt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UpdateDt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1231,7 +1227,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomLeft" activeCell="Q58" sqref="Q58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1260,10 @@
         <v>15</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>9</v>
@@ -1288,7 +1284,7 @@
         <v>70</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M1" s="14" t="s">
         <v>87</v>
@@ -1303,10 +1299,10 @@
         <v>79</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1320,7 +1316,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
@@ -1356,7 +1352,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G3" s="3">
         <v>20</v>
@@ -1371,7 +1367,7 @@
         <v>97</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>97</v>
@@ -1470,13 +1466,13 @@
         <v>20</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>99</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1487,7 +1483,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>23</v>
@@ -1499,13 +1495,13 @@
         <v>20</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>101</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>78</v>
@@ -1647,10 +1643,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M12" s="26">
         <v>1</v>
@@ -1693,7 +1689,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>29</v>
@@ -1713,7 +1709,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>83</v>
@@ -1725,7 +1721,7 @@
         <v>20</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1736,7 +1732,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>28</v>
@@ -1759,7 +1755,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>84</v>
@@ -1787,7 +1783,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>18</v>
@@ -1822,7 +1818,7 @@
         <v>36</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G19" s="3">
         <v>20</v>
@@ -1834,13 +1830,13 @@
         <v>1</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>86</v>
@@ -1895,7 +1891,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>31</v>
@@ -1953,10 +1949,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M23" s="26">
         <v>1</v>
@@ -1976,7 +1972,7 @@
         <v>40</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>29</v>
@@ -1996,7 +1992,7 @@
         <v>40</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>83</v>
@@ -2008,7 +2004,7 @@
         <v>20</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2019,7 +2015,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>28</v>
@@ -2042,7 +2038,7 @@
         <v>40</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>84</v>
@@ -2070,7 +2066,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>18</v>
@@ -2105,7 +2101,7 @@
         <v>59</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G29" s="3">
         <v>20</v>
@@ -2117,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>78</v>
@@ -2178,10 +2174,10 @@
         <v>6</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M31" s="26">
         <v>1</v>
@@ -2201,7 +2197,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>29</v>
@@ -2221,7 +2217,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>83</v>
@@ -2233,7 +2229,7 @@
         <v>20</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2244,7 +2240,7 @@
         <v>56</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>28</v>
@@ -2267,7 +2263,7 @@
         <v>56</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>84</v>
@@ -2297,7 +2293,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>18</v>
@@ -2330,10 +2326,10 @@
         <v>46</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G37" s="3">
         <v>20</v>
@@ -2345,13 +2341,13 @@
         <v>1</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>78</v>
@@ -2406,10 +2402,10 @@
         <v>6</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M39" s="26">
         <v>1</v>
@@ -2429,7 +2425,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>29</v>
@@ -2451,7 +2447,7 @@
         <v>45</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>83</v>
@@ -2473,7 +2469,7 @@
         <v>45</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>28</v>
@@ -2498,7 +2494,7 @@
         <v>45</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>84</v>
@@ -2528,7 +2524,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>18</v>
@@ -2563,7 +2559,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>77</v>
@@ -2599,7 +2595,7 @@
         <v>16</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -2611,13 +2607,13 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G46" s="5">
         <v>20</v>
@@ -2644,7 +2640,7 @@
         <v>78</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -2656,16 +2652,16 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2692,7 +2688,7 @@
         <v>16</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -2704,13 +2700,13 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -2730,7 +2726,7 @@
       </c>
       <c r="P48" s="6"/>
       <c r="R48" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -2742,7 +2738,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>29</v>
@@ -2773,7 +2769,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>83</v>
@@ -2792,7 +2788,7 @@
         <v>89</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
@@ -2806,7 +2802,7 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>28</v>
@@ -2835,7 +2831,7 @@
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>84</v>
@@ -2869,10 +2865,10 @@
         <v>16</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>30</v>
@@ -2884,10 +2880,10 @@
       </c>
       <c r="J53" s="21"/>
       <c r="K53" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L53" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="L53" s="23" t="s">
-        <v>115</v>
       </c>
       <c r="M53" s="26">
         <v>1</v>
@@ -2905,7 +2901,7 @@
         <v>110</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>111</v>
@@ -2914,25 +2910,25 @@
         <v>31</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -2943,37 +2939,37 @@
         <v>110</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L55" s="16" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -2984,10 +2980,10 @@
         <v>110</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>31</v>
@@ -2996,28 +2992,28 @@
         <v>20</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L56" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N56" s="24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q56" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3028,10 +3024,10 @@
         <v>110</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>31</v>
@@ -3040,22 +3036,22 @@
         <v>112</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P57" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -3066,10 +3062,10 @@
         <v>110</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>33</v>
@@ -3099,7 +3095,7 @@
         <v>110</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>29</v>
@@ -3120,10 +3116,10 @@
         <v>110</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>32</v>
@@ -3132,10 +3128,10 @@
         <v>20</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3146,7 +3142,7 @@
         <v>110</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>28</v>
@@ -3166,7 +3162,7 @@
         <v>110</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>84</v>
@@ -3178,7 +3174,7 @@
         <v>7</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62" s="18"/>
@@ -3230,10 +3226,10 @@
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3244,10 +3240,10 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,10 +3254,10 @@
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,10 +3268,10 @@
         <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3286,10 +3282,10 @@
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3300,24 +3296,24 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extract out the parameters as dict object, to reduce the source code.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -635,10 +635,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>seqNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Seq No.</t>
   </si>
   <si>
@@ -735,6 +731,10 @@
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeqNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1223,7 +1223,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M61" sqref="M61"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1296,10 +1296,10 @@
         <v>79</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
@@ -1686,7 +1686,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>29</v>
@@ -1706,7 +1706,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>83</v>
@@ -1729,7 +1729,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>28</v>
@@ -1752,7 +1752,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>84</v>
@@ -1780,7 +1780,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>18</v>
@@ -1969,7 +1969,7 @@
         <v>40</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>29</v>
@@ -1989,7 +1989,7 @@
         <v>40</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>83</v>
@@ -2012,7 +2012,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>28</v>
@@ -2035,7 +2035,7 @@
         <v>40</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>84</v>
@@ -2063,7 +2063,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>18</v>
@@ -2194,7 +2194,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>29</v>
@@ -2214,7 +2214,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>83</v>
@@ -2237,7 +2237,7 @@
         <v>56</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>28</v>
@@ -2260,7 +2260,7 @@
         <v>56</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>84</v>
@@ -2290,7 +2290,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>18</v>
@@ -2422,7 +2422,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>29</v>
@@ -2444,7 +2444,7 @@
         <v>45</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>83</v>
@@ -2466,7 +2466,7 @@
         <v>45</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>28</v>
@@ -2491,7 +2491,7 @@
         <v>45</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>84</v>
@@ -2521,7 +2521,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>18</v>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>77</v>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>139</v>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>140</v>
@@ -2685,7 +2685,7 @@
         <v>16</v>
       </c>
       <c r="R47" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>144</v>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="P48" s="6"/>
       <c r="R48" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>29</v>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>83</v>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>28</v>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>84</v>
@@ -2862,10 +2862,10 @@
         <v>16</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>30</v>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="J53" s="21"/>
       <c r="K53" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L53" s="23" t="s">
         <v>113</v>
@@ -2898,7 +2898,7 @@
         <v>110</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>111</v>
@@ -2907,7 +2907,7 @@
         <v>31</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>125</v>
@@ -2925,7 +2925,7 @@
         <v>16</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>110</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>154</v>
@@ -2945,7 +2945,7 @@
         <v>135</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>126</v>
@@ -2966,7 +2966,7 @@
         <v>118</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -2977,10 +2977,10 @@
         <v>110</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>31</v>
@@ -3010,7 +3010,7 @@
         <v>16</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
         <v>110</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>155</v>
@@ -3033,7 +3033,7 @@
         <v>112</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>127</v>
@@ -3048,7 +3048,7 @@
         <v>16</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>110</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>144</v>
@@ -3092,7 +3092,7 @@
         <v>110</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>29</v>
@@ -3113,10 +3113,10 @@
         <v>110</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>32</v>
@@ -3125,7 +3125,7 @@
         <v>20</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>110</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>28</v>
@@ -3156,7 +3156,7 @@
         <v>110</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>84</v>
@@ -3168,7 +3168,7 @@
         <v>7</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62" s="18"/>

</xml_diff>

<commit_message>
Add isEnable controll template in formEdit.vue file.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="192">
   <si>
     <t>UserId</t>
   </si>
@@ -780,10 +780,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SSSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>spExist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -797,6 +793,22 @@
   </si>
   <si>
     <t>vue-q-input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsEnable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AAAAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>經辦的電腦名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL | 1:是 | 0:否 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1293,7 +1305,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,9 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1389,16 +1401,16 @@
         <v>179</v>
       </c>
       <c r="S1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="T1" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="V1" s="29" t="s">
         <v>186</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -3072,7 +3084,7 @@
         <v>148</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>31</v>
@@ -3114,6 +3126,9 @@
       </c>
       <c r="E55" s="3" t="s">
         <v>105</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>31</v>
@@ -3219,10 +3234,13 @@
         <v>104</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>136</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Kill bad local remote main branch history.
</commit_message>
<xml_diff>
--- a/tableSourceDef.xlsx
+++ b/tableSourceDef.xlsx
@@ -1315,9 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>